<commit_message>
Sorting libraries based on name
</commit_message>
<xml_diff>
--- a/tests/results/dependencies_test.xlsx
+++ b/tests/results/dependencies_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\makge\Python\code_structure\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\makge\Python\codestruct\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
   <si>
     <t>a/a</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>&lt;library&gt;</t>
+  </si>
+  <si>
+    <t>amodule_lib</t>
   </si>
   <si>
     <t>module_lib_1</t>
@@ -1117,7 +1120,9 @@
       <c r="K3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1243,7 +1248,9 @@
       <c r="K4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1369,7 +1376,9 @@
       <c r="K5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1487,15 +1496,17 @@
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1613,15 +1624,17 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1747,7 +1760,9 @@
       <c r="K8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1873,7 +1888,9 @@
       <c r="K9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1999,7 +2016,9 @@
         <v>3</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -2093,18 +2112,40 @@
       <c r="CY10" s="2"/>
     </row>
     <row r="11" spans="1:103" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="B11" s="6">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="C11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="L11" s="1"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>

</xml_diff>